<commit_message>
Tempi e accuratezza integrale openmp
</commit_message>
<xml_diff>
--- a/elaborati_open_mp/elaborato_1/test_accuratezza_integrale.xlsx
+++ b/elaborati_open_mp/elaborato_1/test_accuratezza_integrale.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pa0l0\Downloads\integrale\integrale\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabio/Desktop/CP/GIT/Calcolo-Parallelo/elaborati_open_mp/elaborato_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6F2D9D-03AA-4657-BF0C-78BE18DCAFAC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA1A972-017A-4447-ABD0-D0D8CE5CEB8C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6880" xr2:uid="{6336827A-DD07-43EE-ACE9-D952B3741270}"/>
+    <workbookView xWindow="0" yWindow="7860" windowWidth="18180" windowHeight="12620" xr2:uid="{6336827A-DD07-43EE-ACE9-D952B3741270}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -39,8 +34,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000000000000000"/>
+    <numFmt numFmtId="167" formatCode="0.00000000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -165,8 +161,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -484,21 +480,21 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="25.7265625" customWidth="1"/>
-    <col min="3" max="3" width="23.26953125" customWidth="1"/>
-    <col min="4" max="4" width="20.453125" customWidth="1"/>
-    <col min="5" max="5" width="20.6328125" customWidth="1"/>
-    <col min="6" max="6" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.26953125" customWidth="1"/>
-    <col min="8" max="8" width="19.7265625" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -518,27 +514,27 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>8</v>
       </c>
       <c r="B2" s="8">
-        <v>4.9844573235647402</v>
+        <v>4.9839791881359101</v>
       </c>
       <c r="C2" s="8">
-        <v>4.9840269683880702</v>
+        <v>4.9839791548449304</v>
       </c>
       <c r="D2" s="8">
-        <v>4.9839839358701896</v>
+        <v>4.9839791545120402</v>
       </c>
       <c r="E2" s="8">
-        <v>4.9839796326445098</v>
+        <v>4.9839791545087397</v>
       </c>
       <c r="F2" s="9">
-        <v>4.9839792021280998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+        <v>4.9839791545085603</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C8" s="6"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
@@ -546,7 +542,7 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C9" s="6"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
@@ -554,7 +550,7 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -562,7 +558,7 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -570,7 +566,7 @@
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C12" s="6"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -578,7 +574,7 @@
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C13" s="6"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -586,7 +582,7 @@
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -594,7 +590,7 @@
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>

</xml_diff>